<commit_message>
C# en Noël logboek
C# edit aangepast en clear gefixt zodat hij alleen predictions verwijdert voor ingelogde
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek-Noël.xlsx
+++ b/Documents/Logboeken/Logboek-Noël.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="33">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -508,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,6 +913,58 @@
         <v>3</v>
       </c>
     </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>42866</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="G46" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>42867</v>
+      </c>
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="G49" t="s">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
documentaties en logboek noel
documentaties beter geordend
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek-Noël.xlsx
+++ b/Documents/Logboeken/Logboek-Noël.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="37">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Week 4</t>
+  </si>
+  <si>
+    <t>ziek</t>
+  </si>
+  <si>
+    <t>controleren documentatie</t>
+  </si>
+  <si>
+    <t>Week 5</t>
   </si>
 </sst>
 </file>
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58:I59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1013,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>42863</v>
+        <v>42870</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -1030,7 +1039,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>42864</v>
+        <v>42871</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
@@ -1056,7 +1065,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>42865</v>
+        <v>42872</v>
       </c>
       <c r="B58" t="s">
         <v>33</v>
@@ -1082,7 +1091,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>42866</v>
+        <v>42873</v>
       </c>
       <c r="B61" t="s">
         <v>33</v>
@@ -1093,6 +1102,9 @@
       <c r="E61" s="4"/>
       <c r="G61" t="s">
         <v>3</v>
+      </c>
+      <c r="I61" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -1105,7 +1117,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>42867</v>
+        <v>42874</v>
       </c>
       <c r="B64" t="s">
         <v>33</v>
@@ -1117,14 +1129,164 @@
       <c r="G64" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>33</v>
       </c>
       <c r="G65" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>42884</v>
+      </c>
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="4"/>
+      <c r="G67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="G68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>42885</v>
+      </c>
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="G70" t="s">
+        <v>3</v>
+      </c>
+      <c r="I70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>42886</v>
+      </c>
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="G73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>42887</v>
+      </c>
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="4"/>
+      <c r="G76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>36</v>
+      </c>
+      <c r="G77" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>42888</v>
+      </c>
+      <c r="B79" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" s="4"/>
+      <c r="G79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>36</v>
+      </c>
+      <c r="G80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
documenten en logboek noël
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek-Noël.xlsx
+++ b/Documents/Logboeken/Logboek-Noël.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Week 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentaties aangemaakt </t>
   </si>
 </sst>
 </file>
@@ -529,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,6 +1223,9 @@
       <c r="G73" t="s">
         <v>3</v>
       </c>
+      <c r="I73" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
@@ -1242,6 +1248,9 @@
       <c r="E76" s="4"/>
       <c r="G76" t="s">
         <v>3</v>
+      </c>
+      <c r="I76" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>